<commit_message>
Updated Test cases file and added to finished deliverables
</commit_message>
<xml_diff>
--- a/Finished Deliverables/7-TestCases/TestCases.xlsx
+++ b/Finished Deliverables/7-TestCases/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School Documents\Software Engineering\Deliverables\Deliverables\7-TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UserFiles\Desktop\CurrentClasses\SoftwareEngineering\RIS-Project1\Finished Deliverables\7-TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEB549D-88EC-4A81-9B65-FFC0053BA741}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C23D5-630C-4D43-A15A-785B330CE3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF6808-D506-44CA-A352-BF8FD7553499}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF6808-D506-44CA-A352-BF8FD7553499}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="105">
   <si>
     <t>Test Case</t>
   </si>
@@ -288,25 +288,67 @@
     <t>New data does not appear</t>
   </si>
   <si>
-    <t>Identified typo in updateUser() method parameter</t>
-  </si>
-  <si>
     <t>Identified typo in updateOrder() method parameter</t>
   </si>
   <si>
     <t>Identified typo in updateModality() method parameter</t>
   </si>
   <si>
-    <t>File upload appears in list, but file is not uploaded to RIS Uploads folder. Database is updated.</t>
-  </si>
-  <si>
-    <t>Made changes to uploadFile() method to specify correct upload location</t>
-  </si>
-  <si>
-    <t>Appointment still in Today's Appointments data-table</t>
-  </si>
-  <si>
-    <t>Filter out appointments with checked-in status set to "1"</t>
+    <t>Data appears in data-table, but password is not encrypted until you update the user again.</t>
+  </si>
+  <si>
+    <t>Moved userRepository.save() statement to end of the postMapping(updateUser)</t>
+  </si>
+  <si>
+    <t>Correctly inputs data into Database</t>
+  </si>
+  <si>
+    <t>Price does not appear</t>
+  </si>
+  <si>
+    <t>Error Code 404: Could not establish connection to SQL Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon Scheduling an Appointment the </t>
+  </si>
+  <si>
+    <t>REFERRAL MD - Successful Login</t>
+  </si>
+  <si>
+    <t>Access Denied Splash Screen appears, can not access home page</t>
+  </si>
+  <si>
+    <t>Changed HasAuthority Statements in WebSecurityConfig.java to say Referral_Doctor instead of Referral MD</t>
+  </si>
+  <si>
+    <t>Successful Login for all users except Referral Doctor</t>
+  </si>
+  <si>
+    <t>Successful Login for Referral Doctor</t>
+  </si>
+  <si>
+    <t>Changed application.properties files and added correct credentials and JDBC String</t>
+  </si>
+  <si>
+    <t>RECEPTIONIST - Sending Billing Statement</t>
+  </si>
+  <si>
+    <t>Appointment on Today's Appointment Table and ready to be checked in</t>
+  </si>
+  <si>
+    <t>Returns to Home Screen, Email given on Appointment Scheduling Recieves an Email of Billing Statement</t>
+  </si>
+  <si>
+    <t>Billing Statement not sent, posts to error page</t>
+  </si>
+  <si>
+    <t>Fixed syntax errors for SpringBoot Annotations, mail properties in application.properties, and Java date objects.</t>
+  </si>
+  <si>
+    <t>Error Code 500: Null pointer exception for Insurance information</t>
+  </si>
+  <si>
+    <t>Changed how HTML and ThymeLeaf receive appointment object from AdminController.java</t>
   </si>
 </sst>
 </file>
@@ -560,7 +602,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,9 +613,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -586,9 +625,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -605,6 +641,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -925,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6347CAB-46C1-4AA1-8DCC-06AF9E9DF055}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,634 +1016,662 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="E4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="F33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="C34" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D34" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1604,6 +1689,24 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>